<commit_message>
Merci pour ce moment <3  (Cost des suspensions fini)
</commit_message>
<xml_diff>
--- a/SU - Suspension/Cost/SU_A1500.xlsx
+++ b/SU - Suspension/Cost/SU_A1500.xlsx
@@ -10,14 +10,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="60" windowWidth="16380" windowHeight="8196"/>
+    <workbookView xWindow="4740" yWindow="60" windowWidth="16380" windowHeight="8196" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="8" r:id="rId1"/>
     <sheet name="SU A1500" sheetId="1" r:id="rId2"/>
     <sheet name="SU 1500 001" sheetId="11" r:id="rId3"/>
     <sheet name="dSU 1500 001" sheetId="14" r:id="rId4"/>
-    <sheet name="SU 0600 002" sheetId="10" r:id="rId5"/>
+    <sheet name="SU 1500 002" sheetId="10" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_________uni3">#REF!</definedName>
@@ -86,12 +86,12 @@
     <definedName name="sdf">#REF!</definedName>
     <definedName name="SU_1500_001">'SU 1500 001'!$B$6</definedName>
     <definedName name="SU_1500_001_m">'SU 1500 001'!$N$12</definedName>
-    <definedName name="SU_1500_001_p">'SU 1500 001'!$I$17</definedName>
+    <definedName name="SU_1500_001_p">'SU 1500 001'!$I$18</definedName>
     <definedName name="SU_1500_001_q">'SU 1500 001'!$N$3</definedName>
-    <definedName name="SU_1500_002">'SU 0600 002'!$B$6</definedName>
-    <definedName name="SU_1500_002_m">'SU 0600 002'!$N$12</definedName>
-    <definedName name="SU_1500_002_p">'SU 0600 002'!$I$17</definedName>
-    <definedName name="SU_1500_002_q">'SU 0600 002'!$N$3</definedName>
+    <definedName name="SU_1500_002">'SU 1500 002'!$B$6</definedName>
+    <definedName name="SU_1500_002_m">'SU 1500 002'!$N$12</definedName>
+    <definedName name="SU_1500_002_p">'SU 1500 002'!$I$17</definedName>
+    <definedName name="SU_1500_002_q">'SU 1500 002'!$N$3</definedName>
     <definedName name="SU_A1500">'SU A1500'!$B$5</definedName>
     <definedName name="SU_A1500_f">'SU A1500'!$J$41</definedName>
     <definedName name="SU_A1500_m">'SU A1500'!$N$17</definedName>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="118">
   <si>
     <t>University</t>
   </si>
@@ -469,43 +469,60 @@
   </si>
   <si>
     <t>To tighten the bolts</t>
+  </si>
+  <si>
+    <t>Tapping holes</t>
+  </si>
+  <si>
+    <t>hole</t>
+  </si>
+  <si>
+    <t>Drill &amp; Tap</t>
+  </si>
+  <si>
+    <t>Material removal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="22">
+  <numFmts count="20">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="\$#,##0.00_);&quot;($&quot;#,##0.00\)"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* \-??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00,;_-[$$-409]* \-??_ ;_-@_ "/>
-    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="174" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="175" formatCode="0.0"/>
-    <numFmt numFmtId="176" formatCode="#,##0.000"/>
-    <numFmt numFmtId="177" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.000\);_(\$* \-??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="\$#,##0.00,;&quot;($&quot;#,##0.00\)"/>
-    <numFmt numFmtId="180" formatCode="0.00000000"/>
-    <numFmt numFmtId="184" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="185" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="189" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="193" formatCode="0.000"/>
-    <numFmt numFmtId="222" formatCode="_-* #,##0.0000\ _€_-;\-* #,##0.0000\ _€_-;_-* &quot;-&quot;????????\ _€_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* \-??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00,;_-[$$-409]* \-??_ ;_-@_ "/>
+    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="172" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="173" formatCode="0.0"/>
+    <numFmt numFmtId="174" formatCode="#,##0.000"/>
+    <numFmt numFmtId="175" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.000\);_(\$* \-??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="\$#,##0.00,;&quot;($&quot;#,##0.00\)"/>
+    <numFmt numFmtId="178" formatCode="0.00000000"/>
+    <numFmt numFmtId="179" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="180" formatCode="0.000"/>
+    <numFmt numFmtId="181" formatCode="_-* #,##0.0000\ _€_-;\-* #,##0.0000\ _€_-;_-* &quot;-&quot;????????\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -773,7 +790,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -1268,166 +1285,206 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="56">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="8" fillId="2" borderId="6">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="9" fillId="2" borderId="6">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="1">
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="174" fontId="7" fillId="0" borderId="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="172" fontId="8" fillId="0" borderId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="179" fontId="17" fillId="0" borderId="35">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="28" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="177" fontId="18" fillId="0" borderId="35">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="175" fontId="7" fillId="0" borderId="1">
+    <xf numFmtId="173" fontId="8" fillId="0" borderId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="184" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="185" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="185" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="185" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="185" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="185" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="206">
+  <cellXfs count="212">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="18" fontId="13" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="18" fontId="14" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="13" fillId="0" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="170" fontId="14" fillId="0" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="171" fontId="9" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="14" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="15" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="9" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="12" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="6" borderId="15" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="6" borderId="15" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1438,244 +1495,252 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="37" fontId="6" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="39" fontId="6" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="7" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="39" fontId="7" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="8" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="8"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="6" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="8" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="6" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="6" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="172" fontId="13" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="7" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="171" fontId="14" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="18" fontId="13" fillId="9" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="18" fontId="14" fillId="9" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="3" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="3" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="13" fillId="9" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="171" fontId="14" fillId="9" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="37" fontId="13" fillId="9" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="37" fontId="14" fillId="9" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="172" fontId="13" fillId="9" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="171" fontId="14" fillId="9" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="172" fontId="13" fillId="9" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="14" fillId="9" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="18" fontId="13" fillId="10" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="18" fontId="14" fillId="10" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="3" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="3" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="13" fillId="10" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="171" fontId="14" fillId="10" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="37" fontId="13" fillId="10" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="37" fontId="14" fillId="10" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="172" fontId="13" fillId="10" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="171" fontId="14" fillId="10" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="172" fontId="13" fillId="10" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="14" fillId="10" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="180" fontId="6" fillId="0" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="3" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="8" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="37" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="31" xfId="28" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="32" xfId="28" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="28"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="11"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="28" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="28" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="8" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="37" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" xfId="28" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="32" xfId="28" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="28"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="11"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="28" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="28" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="28" applyFont="1"/>
-    <xf numFmtId="37" fontId="25" fillId="0" borderId="0" xfId="28" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="28" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="23" fillId="12" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="32" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="28" applyFont="1"/>
+    <xf numFmtId="37" fontId="26" fillId="0" borderId="0" xfId="28" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" xfId="28" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="24" fillId="12" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="32" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="31" xfId="28" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="32" xfId="28" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="33" xfId="28" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="34" xfId="28" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="23" fillId="12" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="25" fillId="0" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="30" xfId="28" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="2" xfId="28" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="2" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" xfId="28" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="33" xfId="28" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="34" xfId="28" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="24" fillId="12" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="26" fillId="0" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="30" xfId="28" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="2" xfId="28" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="2" xfId="28" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="25" fillId="0" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="25" fillId="0" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="36" xfId="28" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="174" fontId="26" fillId="0" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="26" fillId="0" borderId="31" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="36" xfId="28" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="38" xfId="28" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="222" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="42" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="11" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="38" xfId="28" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="181" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="42" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="11" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="37" fontId="22" fillId="0" borderId="0" xfId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="37" fontId="23" fillId="0" borderId="0" xfId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="11" fontId="22" fillId="0" borderId="39" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="32" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="23" fillId="0" borderId="39" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="32" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="33" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="11" fontId="22" fillId="0" borderId="0" xfId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="33" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="11" fontId="23" fillId="0" borderId="0" xfId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="193" fontId="22" fillId="0" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="22" fillId="0" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="22" fillId="0" borderId="0" xfId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="23" fillId="0" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="23" fillId="0" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="23" fillId="0" borderId="0" xfId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="29" fillId="0" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="20" fillId="10" borderId="3" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="10" borderId="3" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="51" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="51" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="22" fillId="0" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="51" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="22" fillId="0" borderId="3" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="22" fillId="0" borderId="3" xfId="16" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="189" fontId="22" fillId="0" borderId="3" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="22" fillId="0" borderId="3" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="22" fillId="0" borderId="3" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="3" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="22" fillId="0" borderId="3" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="22" fillId="0" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="51" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="3" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="3" xfId="16" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="23" fillId="0" borderId="3" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="23" fillId="0" borderId="3" xfId="51" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="23" fillId="0" borderId="3" xfId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="3" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="3" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="23" fillId="0" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="41" xfId="28" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="42" xfId="28" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="40" xfId="28" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="40" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="40" xfId="56" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="56">
+  <cellStyles count="57">
     <cellStyle name="Comma 2" xfId="5"/>
     <cellStyle name="Comma 2 2" xfId="21"/>
     <cellStyle name="Comma 2 2 2" xfId="46"/>
@@ -1696,6 +1761,7 @@
     <cellStyle name="Milliers 4" xfId="33"/>
     <cellStyle name="Milliers 5" xfId="17"/>
     <cellStyle name="Milliers 6" xfId="44"/>
+    <cellStyle name="Monétaire" xfId="56" builtinId="4"/>
     <cellStyle name="Monétaire 10" xfId="18"/>
     <cellStyle name="Monétaire 10 2" xfId="29"/>
     <cellStyle name="Monétaire 2" xfId="3"/>
@@ -2245,7 +2311,7 @@
   </sheetPr>
   <dimension ref="A1:O156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H10" sqref="H10"/>
       <selection pane="topRight" activeCell="H10" sqref="H10"/>
@@ -2442,7 +2508,7 @@
       <c r="G8" s="115"/>
       <c r="H8" s="117">
         <f t="shared" si="0"/>
-        <v>0.87618999415608934</v>
+        <v>1.4513899941560895</v>
       </c>
       <c r="I8" s="118">
         <f>SU_1500_001_q</f>
@@ -2454,7 +2520,7 @@
       </c>
       <c r="K8" s="119">
         <f>SU_1500_001_p</f>
-        <v>0.77480000000000004</v>
+        <v>1.35</v>
       </c>
       <c r="L8" s="119">
         <v>0</v>
@@ -2464,7 +2530,7 @@
       </c>
       <c r="N8" s="120">
         <f t="shared" si="1"/>
-        <v>1.7523799883121787</v>
+        <v>2.902779988312179</v>
       </c>
       <c r="O8" s="121"/>
     </row>
@@ -2484,8 +2550,8 @@
       <c r="E9" s="115" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="189" t="str">
-        <f>'SU 0600 002'!B5</f>
+      <c r="F9" s="188" t="str">
+        <f>'SU 1500 002'!B5</f>
         <v>Spacer</v>
       </c>
       <c r="G9" s="115"/>
@@ -2538,7 +2604,7 @@
       </c>
       <c r="K10" s="87">
         <f>SUMPRODUCT($I7:$I9,K7:K9)</f>
-        <v>18.902400000000004</v>
+        <v>20.052800000000001</v>
       </c>
       <c r="L10" s="87">
         <f>SUMPRODUCT($I7:$I9,L7:L9)</f>
@@ -2550,7 +2616,7 @@
       </c>
       <c r="N10" s="87">
         <f>SUM(N7:N9)</f>
-        <v>30.395392942700298</v>
+        <v>31.545792942700299</v>
       </c>
       <c r="O10" s="2"/>
     </row>
@@ -4797,7 +4863,7 @@
   </sheetPr>
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -4863,7 +4929,7 @@
       </c>
       <c r="N2" s="86">
         <f>SU_A1500_pa+SU_A1500_m+SU_A1500_p+SU_A1500_f</f>
-        <v>15.197696471350149</v>
+        <v>15.772896471350148</v>
       </c>
       <c r="O2" s="61"/>
     </row>
@@ -4939,7 +5005,7 @@
       </c>
       <c r="N5" s="73">
         <f>N2*SU_A1500_q</f>
-        <v>30.395392942700298</v>
+        <v>31.545792942700295</v>
       </c>
       <c r="O5" s="61"/>
     </row>
@@ -5040,14 +5106,14 @@
       </c>
       <c r="C10" s="31">
         <f>'SU 1500 001'!N2</f>
-        <v>0.87618999415608934</v>
+        <v>1.4513899941560895</v>
       </c>
       <c r="D10" s="130">
         <v>1</v>
       </c>
       <c r="E10" s="31">
         <f>C10*D10</f>
-        <v>0.87618999415608934</v>
+        <v>1.4513899941560895</v>
       </c>
       <c r="F10" s="55"/>
       <c r="G10" s="55"/>
@@ -5068,7 +5134,7 @@
         <v>83</v>
       </c>
       <c r="C11" s="31">
-        <f>'SU 0600 002'!N2</f>
+        <f>'SU 1500 002'!N2</f>
         <v>0.26540753801370742</v>
       </c>
       <c r="D11" s="19">
@@ -5098,7 +5164,7 @@
       </c>
       <c r="E12" s="93">
         <f>SUM(E10:E11)</f>
-        <v>1.937820146210919</v>
+        <v>2.513020146210919</v>
       </c>
       <c r="F12" s="56"/>
       <c r="G12" s="56"/>
@@ -5177,34 +5243,34 @@
       <c r="A15" s="71">
         <v>10</v>
       </c>
-      <c r="B15" s="197" t="s">
+      <c r="B15" s="196" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="197" t="s">
+      <c r="C15" s="196" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="196">
+      <c r="D15" s="195">
         <f>0.02*E15^2+1.22</f>
         <v>2.5</v>
       </c>
-      <c r="E15" s="197">
+      <c r="E15" s="196">
         <v>8</v>
       </c>
-      <c r="F15" s="197" t="s">
+      <c r="F15" s="196" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="197"/>
-      <c r="H15" s="199"/>
-      <c r="I15" s="201" t="s">
+      <c r="G15" s="196"/>
+      <c r="H15" s="198"/>
+      <c r="I15" s="200" t="s">
         <v>95</v>
       </c>
-      <c r="J15" s="200"/>
-      <c r="K15" s="199"/>
-      <c r="L15" s="199"/>
-      <c r="M15" s="200">
+      <c r="J15" s="199"/>
+      <c r="K15" s="198"/>
+      <c r="L15" s="198"/>
+      <c r="M15" s="199">
         <v>1</v>
       </c>
-      <c r="N15" s="198">
+      <c r="N15" s="197">
         <f>D15*M15</f>
         <v>2.5</v>
       </c>
@@ -5214,34 +5280,34 @@
       <c r="A16" s="71">
         <v>20</v>
       </c>
-      <c r="B16" s="197" t="s">
+      <c r="B16" s="196" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="197" t="s">
+      <c r="C16" s="196" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="205">
+      <c r="D16" s="204">
         <f>0.02*E16^2+1.22</f>
         <v>2.5</v>
       </c>
-      <c r="E16" s="197">
+      <c r="E16" s="196">
         <v>8</v>
       </c>
-      <c r="F16" s="197" t="s">
+      <c r="F16" s="196" t="s">
         <v>30</v>
       </c>
-      <c r="G16" s="197"/>
-      <c r="H16" s="199"/>
-      <c r="I16" s="203" t="s">
+      <c r="G16" s="196"/>
+      <c r="H16" s="198"/>
+      <c r="I16" s="202" t="s">
         <v>95</v>
       </c>
-      <c r="J16" s="200"/>
-      <c r="K16" s="199"/>
-      <c r="L16" s="202"/>
-      <c r="M16" s="200">
+      <c r="J16" s="199"/>
+      <c r="K16" s="198"/>
+      <c r="L16" s="201"/>
+      <c r="M16" s="199">
         <v>1</v>
       </c>
-      <c r="N16" s="204">
+      <c r="N16" s="203">
         <f>D16*M16</f>
         <v>2.5</v>
       </c>
@@ -5249,7 +5315,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="66"/>
-      <c r="B17" s="195" t="s">
+      <c r="B17" s="194" t="s">
         <v>102</v>
       </c>
       <c r="C17" s="25"/>
@@ -5327,10 +5393,10 @@
       <c r="A20" s="71">
         <v>10</v>
       </c>
-      <c r="B20" s="194" t="s">
+      <c r="B20" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="193" t="s">
+      <c r="C20" s="192" t="s">
         <v>98</v>
       </c>
       <c r="D20" s="72">
@@ -5361,16 +5427,16 @@
       <c r="A21" s="71">
         <v>20</v>
       </c>
-      <c r="B21" s="194" t="s">
+      <c r="B21" s="193" t="s">
         <v>99</v>
       </c>
-      <c r="C21" s="193" t="s">
+      <c r="C21" s="192" t="s">
         <v>100</v>
       </c>
       <c r="D21" s="72">
         <v>0.5</v>
       </c>
-      <c r="E21" s="192" t="s">
+      <c r="E21" s="191" t="s">
         <v>35</v>
       </c>
       <c r="F21" s="71">
@@ -5395,10 +5461,10 @@
       <c r="A22" s="71">
         <v>30</v>
       </c>
-      <c r="B22" s="194" t="s">
+      <c r="B22" s="193" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="193" t="s">
+      <c r="C22" s="192" t="s">
         <v>67</v>
       </c>
       <c r="D22" s="72">
@@ -5429,10 +5495,10 @@
       <c r="A23" s="71">
         <v>40</v>
       </c>
-      <c r="B23" s="194" t="s">
+      <c r="B23" s="193" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="193" t="s">
+      <c r="C23" s="192" t="s">
         <v>67</v>
       </c>
       <c r="D23" s="72">
@@ -5463,23 +5529,23 @@
       <c r="A24" s="71">
         <v>50</v>
       </c>
-      <c r="B24" s="193" t="s">
+      <c r="B24" s="192" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="193" t="s">
+      <c r="C24" s="192" t="s">
         <v>105</v>
       </c>
-      <c r="D24" s="191">
+      <c r="D24" s="190">
         <v>0.06</v>
       </c>
-      <c r="E24" s="190" t="s">
+      <c r="E24" s="189" t="s">
         <v>35</v>
       </c>
-      <c r="F24" s="190">
+      <c r="F24" s="189">
         <v>2</v>
       </c>
-      <c r="G24" s="190"/>
-      <c r="H24" s="190">
+      <c r="G24" s="189"/>
+      <c r="H24" s="189">
         <v>1</v>
       </c>
       <c r="I24" s="72">
@@ -5497,23 +5563,23 @@
       <c r="A25" s="128">
         <v>60</v>
       </c>
-      <c r="B25" s="193" t="s">
+      <c r="B25" s="192" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="193" t="s">
+      <c r="C25" s="192" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="191">
+      <c r="D25" s="190">
         <v>0.06</v>
       </c>
-      <c r="E25" s="190" t="s">
+      <c r="E25" s="189" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="190">
+      <c r="F25" s="189">
         <v>2</v>
       </c>
-      <c r="G25" s="190"/>
-      <c r="H25" s="190">
+      <c r="G25" s="189"/>
+      <c r="H25" s="189">
         <v>1</v>
       </c>
       <c r="I25" s="72">
@@ -5532,23 +5598,23 @@
         <f>A25+10</f>
         <v>70</v>
       </c>
-      <c r="B26" s="194" t="s">
+      <c r="B26" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="193" t="s">
+      <c r="C26" s="192" t="s">
         <v>106</v>
       </c>
-      <c r="D26" s="191">
+      <c r="D26" s="190">
         <v>0.12</v>
       </c>
-      <c r="E26" s="190" t="s">
+      <c r="E26" s="189" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="190">
+      <c r="F26" s="189">
         <v>1</v>
       </c>
-      <c r="G26" s="190"/>
-      <c r="H26" s="190">
+      <c r="G26" s="189"/>
+      <c r="H26" s="189">
         <v>1</v>
       </c>
       <c r="I26" s="72">
@@ -5567,23 +5633,23 @@
         <f t="shared" ref="A27:A32" si="1">A26+10</f>
         <v>80</v>
       </c>
-      <c r="B27" s="190" t="s">
+      <c r="B27" s="189" t="s">
         <v>103</v>
       </c>
-      <c r="C27" s="193" t="s">
+      <c r="C27" s="192" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="191">
+      <c r="D27" s="190">
         <v>0.06</v>
       </c>
-      <c r="E27" s="190" t="s">
+      <c r="E27" s="189" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="190">
+      <c r="F27" s="189">
         <v>2</v>
       </c>
-      <c r="G27" s="190"/>
-      <c r="H27" s="190">
+      <c r="G27" s="189"/>
+      <c r="H27" s="189">
         <v>1</v>
       </c>
       <c r="I27" s="72">
@@ -5602,23 +5668,23 @@
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="B28" s="190" t="s">
+      <c r="B28" s="189" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="193" t="s">
+      <c r="C28" s="192" t="s">
         <v>108</v>
       </c>
-      <c r="D28" s="191">
+      <c r="D28" s="190">
         <v>0.06</v>
       </c>
-      <c r="E28" s="190" t="s">
+      <c r="E28" s="189" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="190">
+      <c r="F28" s="189">
         <v>2</v>
       </c>
-      <c r="G28" s="190"/>
-      <c r="H28" s="190">
+      <c r="G28" s="189"/>
+      <c r="H28" s="189">
         <v>1</v>
       </c>
       <c r="I28" s="72">
@@ -5637,23 +5703,23 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="B29" s="194" t="s">
+      <c r="B29" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="193" t="s">
+      <c r="C29" s="192" t="s">
         <v>109</v>
       </c>
-      <c r="D29" s="191">
+      <c r="D29" s="190">
         <v>0.12</v>
       </c>
-      <c r="E29" s="190" t="s">
+      <c r="E29" s="189" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="190">
+      <c r="F29" s="189">
         <v>1</v>
       </c>
-      <c r="G29" s="190"/>
-      <c r="H29" s="190">
+      <c r="G29" s="189"/>
+      <c r="H29" s="189">
         <v>1</v>
       </c>
       <c r="I29" s="72">
@@ -5672,23 +5738,23 @@
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="B30" s="194" t="s">
+      <c r="B30" s="193" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="193" t="s">
+      <c r="C30" s="192" t="s">
         <v>104</v>
       </c>
-      <c r="D30" s="191">
+      <c r="D30" s="190">
         <v>0.12</v>
       </c>
-      <c r="E30" s="190" t="s">
+      <c r="E30" s="189" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="190">
+      <c r="F30" s="189">
         <v>2</v>
       </c>
-      <c r="G30" s="190"/>
-      <c r="H30" s="190">
+      <c r="G30" s="189"/>
+      <c r="H30" s="189">
         <v>1</v>
       </c>
       <c r="I30" s="72">
@@ -5707,23 +5773,23 @@
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="B31" s="194" t="s">
+      <c r="B31" s="193" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="193" t="s">
+      <c r="C31" s="192" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="191">
+      <c r="D31" s="190">
         <v>0.75</v>
       </c>
-      <c r="E31" s="190" t="s">
+      <c r="E31" s="189" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="190">
+      <c r="F31" s="189">
         <v>2</v>
       </c>
-      <c r="G31" s="190"/>
-      <c r="H31" s="190">
+      <c r="G31" s="189"/>
+      <c r="H31" s="189">
         <v>1</v>
       </c>
       <c r="I31" s="72">
@@ -5742,23 +5808,23 @@
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="B32" s="194" t="s">
+      <c r="B32" s="193" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="193" t="s">
+      <c r="C32" s="192" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="191">
+      <c r="D32" s="190">
         <v>0.25</v>
       </c>
-      <c r="E32" s="190" t="s">
+      <c r="E32" s="189" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="190">
+      <c r="F32" s="189">
         <v>2</v>
       </c>
-      <c r="G32" s="190"/>
-      <c r="H32" s="190">
+      <c r="G32" s="189"/>
+      <c r="H32" s="189">
         <v>1</v>
       </c>
       <c r="I32" s="72">
@@ -6125,10 +6191,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A2:N280"/>
+  <dimension ref="A2:N281"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6141,7 +6207,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="153" t="s">
+      <c r="A2" s="152" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="16" t="s">
@@ -6156,23 +6222,23 @@
       <c r="G2" s="136"/>
       <c r="H2" s="136"/>
       <c r="I2" s="136"/>
-      <c r="J2" s="154" t="s">
+      <c r="J2" s="153" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="137">
         <v>81</v>
       </c>
       <c r="L2" s="136"/>
-      <c r="M2" s="153" t="s">
+      <c r="M2" s="152" t="s">
         <v>16</v>
       </c>
       <c r="N2" s="140">
         <f>SU_1500_001_m+SU_1500_001_p</f>
-        <v>0.87618999415608934</v>
+        <v>1.4513899941560895</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="152" t="s">
+      <c r="A3" s="151" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="16" t="str">
@@ -6180,7 +6246,7 @@
         <v>Suspension &amp; Shocks</v>
       </c>
       <c r="C3" s="136"/>
-      <c r="D3" s="153" t="s">
+      <c r="D3" s="152" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="82" t="s">
@@ -6193,7 +6259,7 @@
       <c r="J3" s="136"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
-      <c r="M3" s="152" t="s">
+      <c r="M3" s="151" t="s">
         <v>4</v>
       </c>
       <c r="N3" s="139">
@@ -6201,7 +6267,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="152" t="s">
+      <c r="A4" s="151" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="81" t="str">
@@ -6209,7 +6275,7 @@
         <v>Rear Pushrod</v>
       </c>
       <c r="C4" s="136"/>
-      <c r="D4" s="152" t="s">
+      <c r="D4" s="151" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="136"/>
@@ -6217,7 +6283,7 @@
       <c r="G4" s="136"/>
       <c r="H4" s="136"/>
       <c r="I4" s="136"/>
-      <c r="J4" s="153" t="s">
+      <c r="J4" s="152" t="s">
         <v>6</v>
       </c>
       <c r="K4" s="136"/>
@@ -6226,14 +6292,14 @@
       <c r="N4" s="136"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="152" t="s">
+      <c r="A5" s="151" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="125" t="s">
         <v>92</v>
       </c>
       <c r="C5" s="136"/>
-      <c r="D5" s="152" t="s">
+      <c r="D5" s="151" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="136"/>
@@ -6241,21 +6307,21 @@
       <c r="G5" s="136"/>
       <c r="H5" s="136"/>
       <c r="I5" s="136"/>
-      <c r="J5" s="152" t="s">
+      <c r="J5" s="151" t="s">
         <v>8</v>
       </c>
       <c r="K5" s="136"/>
       <c r="L5" s="136"/>
-      <c r="M5" s="153" t="s">
+      <c r="M5" s="152" t="s">
         <v>9</v>
       </c>
       <c r="N5" s="140">
         <f>N2*SU_1500_001_q</f>
-        <v>1.7523799883121787</v>
+        <v>2.902779988312179</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="152" t="s">
+      <c r="A6" s="151" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="124" t="s">
@@ -6268,7 +6334,7 @@
       <c r="G6" s="136"/>
       <c r="H6" s="136"/>
       <c r="I6" s="136"/>
-      <c r="J6" s="152" t="s">
+      <c r="J6" s="151" t="s">
         <v>12</v>
       </c>
       <c r="K6" s="136"/>
@@ -6277,7 +6343,7 @@
       <c r="N6" s="136"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="152" t="s">
+      <c r="A7" s="151" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="16" t="s">
@@ -6297,7 +6363,7 @@
       <c r="N7" s="136"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="152" t="s">
+      <c r="A8" s="151" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="16"/>
@@ -6331,63 +6397,63 @@
       <c r="N9" s="136"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="147" t="s">
+      <c r="A10" s="146" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="146" t="s">
+      <c r="B10" s="145" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="146" t="s">
+      <c r="C10" s="145" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="146" t="s">
+      <c r="D10" s="145" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="146" t="s">
+      <c r="E10" s="145" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="146" t="s">
+      <c r="F10" s="145" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="146" t="s">
+      <c r="G10" s="145" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="146" t="s">
+      <c r="H10" s="145" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="146" t="s">
+      <c r="I10" s="145" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="146" t="s">
+      <c r="J10" s="145" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="146" t="s">
+      <c r="K10" s="145" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="146" t="s">
+      <c r="L10" s="145" t="s">
         <v>29</v>
       </c>
-      <c r="M10" s="146" t="s">
+      <c r="M10" s="145" t="s">
         <v>17</v>
       </c>
-      <c r="N10" s="146" t="s">
+      <c r="N10" s="145" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="157">
+      <c r="A11" s="156">
         <v>10</v>
       </c>
-      <c r="B11" s="158" t="s">
+      <c r="B11" s="157" t="s">
         <v>88</v>
       </c>
-      <c r="C11" s="159" t="s">
+      <c r="C11" s="158" t="s">
         <v>90</v>
       </c>
       <c r="D11" s="143">
         <v>2.25</v>
       </c>
-      <c r="E11" s="156">
+      <c r="E11" s="155">
         <f>J11*K11*L11</f>
         <v>4.5062219624928589E-2</v>
       </c>
@@ -6395,21 +6461,21 @@
         <v>71</v>
       </c>
       <c r="G11" s="144"/>
-      <c r="H11" s="150"/>
-      <c r="I11" s="151" t="s">
+      <c r="H11" s="149"/>
+      <c r="I11" s="150" t="s">
         <v>89</v>
       </c>
-      <c r="J11" s="151">
+      <c r="J11" s="150">
         <f>PI()*(7.5*10^-3)^2</f>
         <v>1.7671458676442585E-4</v>
       </c>
-      <c r="K11" s="155">
+      <c r="K11" s="154">
         <v>0.03</v>
       </c>
-      <c r="L11" s="149">
+      <c r="L11" s="148">
         <v>8500</v>
       </c>
-      <c r="M11" s="149">
+      <c r="M11" s="148">
         <v>1</v>
       </c>
       <c r="N11" s="143">
@@ -6433,7 +6499,7 @@
       <c r="M12" s="142" t="s">
         <v>18</v>
       </c>
-      <c r="N12" s="148">
+      <c r="N12" s="147">
         <f>N11</f>
         <v>0.10138999415608932</v>
       </c>
@@ -6455,31 +6521,31 @@
       <c r="N13" s="136"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="147" t="s">
+      <c r="A14" s="205" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="146" t="s">
+      <c r="B14" s="206" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="146" t="s">
+      <c r="C14" s="206" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="146" t="s">
+      <c r="D14" s="206" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="146" t="s">
+      <c r="E14" s="206" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="146" t="s">
+      <c r="F14" s="206" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="146" t="s">
+      <c r="G14" s="206" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="146" t="s">
+      <c r="H14" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="146" t="s">
+      <c r="I14" s="206" t="s">
         <v>18</v>
       </c>
       <c r="J14" s="138"/>
@@ -6489,29 +6555,29 @@
       <c r="N14" s="138"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="145">
+      <c r="A15" s="207">
         <v>10</v>
       </c>
-      <c r="B15" s="144" t="s">
+      <c r="B15" s="207" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="144"/>
-      <c r="D15" s="143">
+      <c r="C15" s="207"/>
+      <c r="D15" s="208">
         <v>1.3</v>
       </c>
-      <c r="E15" s="144" t="s">
+      <c r="E15" s="207" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="144">
+      <c r="F15" s="207">
         <v>1</v>
       </c>
-      <c r="G15" s="144" t="s">
+      <c r="G15" s="207" t="s">
         <v>78</v>
       </c>
-      <c r="H15" s="144">
+      <c r="H15" s="207">
         <v>0.5</v>
       </c>
-      <c r="I15" s="143">
+      <c r="I15" s="208">
         <f>D15*H15*F15</f>
         <v>0.65</v>
       </c>
@@ -6522,31 +6588,31 @@
       <c r="N15" s="136"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="145">
+      <c r="A16" s="207">
         <v>20</v>
       </c>
-      <c r="B16" s="144" t="s">
+      <c r="B16" s="207" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="144" t="s">
+      <c r="C16" s="207" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="143">
+      <c r="D16" s="208">
         <v>0.04</v>
       </c>
-      <c r="E16" s="144" t="s">
+      <c r="E16" s="207" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="144">
+      <c r="F16" s="207">
         <v>1.04</v>
       </c>
-      <c r="G16" s="144" t="s">
+      <c r="G16" s="207" t="s">
         <v>73</v>
       </c>
-      <c r="H16" s="144">
+      <c r="H16" s="207">
         <v>3</v>
       </c>
-      <c r="I16" s="143">
+      <c r="I16" s="208">
         <f>D16*F16*H16</f>
         <v>0.12480000000000002</v>
       </c>
@@ -6557,41 +6623,60 @@
       <c r="N16" s="136"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="138"/>
-      <c r="B17" s="138"/>
-      <c r="C17" s="138"/>
-      <c r="D17" s="138"/>
-      <c r="E17" s="138"/>
-      <c r="F17" s="138"/>
-      <c r="G17" s="138"/>
-      <c r="H17" s="142" t="s">
+      <c r="A17" s="207">
+        <v>30</v>
+      </c>
+      <c r="B17" s="209" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="210" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="208">
+        <v>0.35</v>
+      </c>
+      <c r="E17" s="209" t="s">
+        <v>115</v>
+      </c>
+      <c r="F17" s="209">
+        <v>2</v>
+      </c>
+      <c r="G17" s="209" t="s">
+        <v>116</v>
+      </c>
+      <c r="H17" s="211">
+        <v>1</v>
+      </c>
+      <c r="I17" s="208">
+        <f>D17*F17*H17</f>
+        <v>0.7</v>
+      </c>
+      <c r="J17" s="136"/>
+      <c r="K17" s="136"/>
+      <c r="L17" s="136"/>
+      <c r="M17" s="136"/>
+      <c r="N17" s="136"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="138"/>
+      <c r="B18" s="138"/>
+      <c r="C18" s="138"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="138"/>
+      <c r="F18" s="138"/>
+      <c r="G18" s="138"/>
+      <c r="H18" s="142" t="s">
         <v>18</v>
       </c>
-      <c r="I17" s="141">
-        <f>I15+I16</f>
-        <v>0.77480000000000004</v>
-      </c>
-      <c r="J17" s="138"/>
-      <c r="K17" s="138"/>
-      <c r="L17" s="138"/>
-      <c r="M17" s="138"/>
-      <c r="N17" s="138"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="136"/>
-      <c r="B18" s="136"/>
-      <c r="C18" s="136"/>
-      <c r="D18" s="136"/>
-      <c r="E18" s="136"/>
-      <c r="F18" s="136"/>
-      <c r="G18" s="136"/>
-      <c r="H18" s="137"/>
-      <c r="I18" s="140"/>
-      <c r="J18" s="136"/>
-      <c r="K18" s="136"/>
-      <c r="L18" s="136"/>
-      <c r="M18" s="136"/>
-      <c r="N18" s="136"/>
+      <c r="I18" s="141">
+        <f>I15+I17</f>
+        <v>1.35</v>
+      </c>
+      <c r="J18" s="138"/>
+      <c r="K18" s="138"/>
+      <c r="L18" s="138"/>
+      <c r="M18" s="138"/>
+      <c r="N18" s="138"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="136"/>
@@ -6601,8 +6686,8 @@
       <c r="E19" s="136"/>
       <c r="F19" s="136"/>
       <c r="G19" s="136"/>
-      <c r="H19" s="136"/>
-      <c r="I19" s="136"/>
+      <c r="H19" s="137"/>
+      <c r="I19" s="140"/>
       <c r="J19" s="136"/>
       <c r="K19" s="136"/>
       <c r="L19" s="136"/>
@@ -6658,7 +6743,7 @@
       <c r="N22" s="136"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="16"/>
+      <c r="A23" s="136"/>
       <c r="B23" s="136"/>
       <c r="C23" s="136"/>
       <c r="D23" s="136"/>
@@ -6690,7 +6775,7 @@
       <c r="N24" s="136"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A25" s="81"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="136"/>
       <c r="C25" s="136"/>
       <c r="D25" s="136"/>
@@ -6706,7 +6791,7 @@
       <c r="N25" s="136"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
+      <c r="A26" s="81"/>
       <c r="B26" s="136"/>
       <c r="C26" s="136"/>
       <c r="D26" s="136"/>
@@ -6722,7 +6807,7 @@
       <c r="N26" s="136"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="27"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="136"/>
       <c r="C27" s="136"/>
       <c r="D27" s="136"/>
@@ -6738,7 +6823,7 @@
       <c r="N27" s="136"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A28" s="16"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="136"/>
       <c r="C28" s="136"/>
       <c r="D28" s="136"/>
@@ -6770,7 +6855,7 @@
       <c r="N29" s="136"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" s="136"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="136"/>
       <c r="C30" s="136"/>
       <c r="D30" s="136"/>
@@ -9643,11 +9728,11 @@
       <c r="G209" s="136"/>
       <c r="H209" s="136"/>
       <c r="I209" s="136"/>
-      <c r="J209" s="134"/>
-      <c r="K209" s="134"/>
-      <c r="L209" s="134"/>
-      <c r="M209" s="134"/>
-      <c r="N209" s="134"/>
+      <c r="J209" s="136"/>
+      <c r="K209" s="136"/>
+      <c r="L209" s="136"/>
+      <c r="M209" s="136"/>
+      <c r="N209" s="136"/>
     </row>
     <row r="210" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A210" s="136"/>
@@ -9659,6 +9744,11 @@
       <c r="G210" s="136"/>
       <c r="H210" s="136"/>
       <c r="I210" s="136"/>
+      <c r="J210" s="134"/>
+      <c r="K210" s="134"/>
+      <c r="L210" s="134"/>
+      <c r="M210" s="134"/>
+      <c r="N210" s="134"/>
     </row>
     <row r="211" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A211" s="136"/>
@@ -10429,6 +10519,17 @@
       <c r="G280" s="136"/>
       <c r="H280" s="136"/>
       <c r="I280" s="136"/>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A281" s="136"/>
+      <c r="B281" s="136"/>
+      <c r="C281" s="136"/>
+      <c r="D281" s="136"/>
+      <c r="E281" s="136"/>
+      <c r="F281" s="136"/>
+      <c r="G281" s="136"/>
+      <c r="H281" s="136"/>
+      <c r="I281" s="136"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -10483,7 +10584,7 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10767,7 +10868,7 @@
       <c r="D11" s="31">
         <v>2.25</v>
       </c>
-      <c r="E11" s="160">
+      <c r="E11" s="159">
         <f>L11*J11*K11</f>
         <v>9.4700168949810714E-3</v>
       </c>
@@ -10776,7 +10877,7 @@
       </c>
       <c r="G11" s="21"/>
       <c r="H11" s="20"/>
-      <c r="I11" s="168" t="s">
+      <c r="I11" s="167" t="s">
         <v>86</v>
       </c>
       <c r="J11" s="123">
@@ -10983,344 +11084,344 @@
       <c r="O18" s="70"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="178"/>
-      <c r="B22" s="178"/>
-      <c r="C22" s="178"/>
-      <c r="D22" s="178"/>
-      <c r="E22" s="178"/>
-      <c r="F22" s="178"/>
-      <c r="G22" s="178"/>
-      <c r="H22" s="178"/>
-      <c r="I22" s="178"/>
-      <c r="J22" s="178"/>
-      <c r="K22" s="178"/>
-      <c r="L22" s="178"/>
-      <c r="M22" s="178"/>
-      <c r="N22" s="178"/>
-      <c r="O22" s="178"/>
-      <c r="P22" s="178"/>
+      <c r="A22" s="177"/>
+      <c r="B22" s="177"/>
+      <c r="C22" s="177"/>
+      <c r="D22" s="177"/>
+      <c r="E22" s="177"/>
+      <c r="F22" s="177"/>
+      <c r="G22" s="177"/>
+      <c r="H22" s="177"/>
+      <c r="I22" s="177"/>
+      <c r="J22" s="177"/>
+      <c r="K22" s="177"/>
+      <c r="L22" s="177"/>
+      <c r="M22" s="177"/>
+      <c r="N22" s="177"/>
+      <c r="O22" s="177"/>
+      <c r="P22" s="177"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="178"/>
-      <c r="B23" s="169"/>
-      <c r="C23" s="163"/>
-      <c r="D23" s="163"/>
-      <c r="E23" s="163"/>
-      <c r="F23" s="163"/>
-      <c r="G23" s="162"/>
-      <c r="H23" s="163"/>
-      <c r="I23" s="163"/>
-      <c r="J23" s="163"/>
-      <c r="K23" s="179"/>
-      <c r="L23" s="164"/>
-      <c r="M23" s="163"/>
-      <c r="N23" s="169"/>
-      <c r="O23" s="165"/>
-      <c r="P23" s="178"/>
+      <c r="A23" s="177"/>
+      <c r="B23" s="168"/>
+      <c r="C23" s="162"/>
+      <c r="D23" s="162"/>
+      <c r="E23" s="162"/>
+      <c r="F23" s="162"/>
+      <c r="G23" s="161"/>
+      <c r="H23" s="162"/>
+      <c r="I23" s="162"/>
+      <c r="J23" s="162"/>
+      <c r="K23" s="178"/>
+      <c r="L23" s="163"/>
+      <c r="M23" s="162"/>
+      <c r="N23" s="168"/>
+      <c r="O23" s="164"/>
+      <c r="P23" s="177"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="178"/>
-      <c r="B24" s="169"/>
-      <c r="C24" s="163"/>
-      <c r="D24" s="180"/>
-      <c r="E24" s="162"/>
-      <c r="F24" s="163"/>
-      <c r="G24" s="163"/>
-      <c r="H24" s="163"/>
-      <c r="I24" s="163"/>
-      <c r="J24" s="163"/>
-      <c r="K24" s="163"/>
-      <c r="L24" s="163"/>
-      <c r="M24" s="163"/>
-      <c r="N24" s="169"/>
-      <c r="O24" s="166"/>
-      <c r="P24" s="178"/>
+      <c r="A24" s="177"/>
+      <c r="B24" s="168"/>
+      <c r="C24" s="162"/>
+      <c r="D24" s="179"/>
+      <c r="E24" s="161"/>
+      <c r="F24" s="162"/>
+      <c r="G24" s="162"/>
+      <c r="H24" s="162"/>
+      <c r="I24" s="162"/>
+      <c r="J24" s="162"/>
+      <c r="K24" s="162"/>
+      <c r="L24" s="162"/>
+      <c r="M24" s="162"/>
+      <c r="N24" s="168"/>
+      <c r="O24" s="165"/>
+      <c r="P24" s="177"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="178"/>
-      <c r="B25" s="169"/>
-      <c r="C25" s="162"/>
-      <c r="D25" s="163"/>
-      <c r="E25" s="169"/>
-      <c r="F25" s="163"/>
-      <c r="G25" s="163"/>
-      <c r="H25" s="163"/>
-      <c r="I25" s="163"/>
-      <c r="J25" s="163"/>
-      <c r="K25" s="169"/>
-      <c r="L25" s="163"/>
-      <c r="M25" s="163"/>
-      <c r="N25" s="163"/>
-      <c r="O25" s="161"/>
-      <c r="P25" s="178"/>
+      <c r="A25" s="177"/>
+      <c r="B25" s="168"/>
+      <c r="C25" s="161"/>
+      <c r="D25" s="162"/>
+      <c r="E25" s="168"/>
+      <c r="F25" s="162"/>
+      <c r="G25" s="162"/>
+      <c r="H25" s="162"/>
+      <c r="I25" s="162"/>
+      <c r="J25" s="162"/>
+      <c r="K25" s="168"/>
+      <c r="L25" s="162"/>
+      <c r="M25" s="162"/>
+      <c r="N25" s="162"/>
+      <c r="O25" s="160"/>
+      <c r="P25" s="177"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="178"/>
-      <c r="B26" s="169"/>
-      <c r="C26" s="171"/>
-      <c r="D26" s="163"/>
-      <c r="E26" s="169"/>
-      <c r="F26" s="163"/>
-      <c r="G26" s="163"/>
-      <c r="H26" s="163"/>
-      <c r="I26" s="163"/>
-      <c r="J26" s="163"/>
-      <c r="K26" s="169"/>
-      <c r="L26" s="163"/>
-      <c r="M26" s="163"/>
-      <c r="N26" s="169"/>
-      <c r="O26" s="165"/>
-      <c r="P26" s="178"/>
+      <c r="A26" s="177"/>
+      <c r="B26" s="168"/>
+      <c r="C26" s="170"/>
+      <c r="D26" s="162"/>
+      <c r="E26" s="168"/>
+      <c r="F26" s="162"/>
+      <c r="G26" s="162"/>
+      <c r="H26" s="162"/>
+      <c r="I26" s="162"/>
+      <c r="J26" s="162"/>
+      <c r="K26" s="168"/>
+      <c r="L26" s="162"/>
+      <c r="M26" s="162"/>
+      <c r="N26" s="168"/>
+      <c r="O26" s="164"/>
+      <c r="P26" s="177"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="178"/>
-      <c r="B27" s="169"/>
-      <c r="C27" s="167"/>
-      <c r="D27" s="163"/>
-      <c r="E27" s="163"/>
-      <c r="F27" s="163"/>
-      <c r="G27" s="163"/>
-      <c r="H27" s="163"/>
-      <c r="I27" s="163"/>
-      <c r="J27" s="163"/>
-      <c r="K27" s="169"/>
-      <c r="L27" s="163"/>
-      <c r="M27" s="163"/>
-      <c r="N27" s="163"/>
-      <c r="O27" s="163"/>
-      <c r="P27" s="178"/>
+      <c r="A27" s="177"/>
+      <c r="B27" s="168"/>
+      <c r="C27" s="166"/>
+      <c r="D27" s="162"/>
+      <c r="E27" s="162"/>
+      <c r="F27" s="162"/>
+      <c r="G27" s="162"/>
+      <c r="H27" s="162"/>
+      <c r="I27" s="162"/>
+      <c r="J27" s="162"/>
+      <c r="K27" s="168"/>
+      <c r="L27" s="162"/>
+      <c r="M27" s="162"/>
+      <c r="N27" s="162"/>
+      <c r="O27" s="162"/>
+      <c r="P27" s="177"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="178"/>
-      <c r="B28" s="169"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="163"/>
-      <c r="L28" s="163"/>
-      <c r="M28" s="163"/>
-      <c r="N28" s="163"/>
-      <c r="O28" s="163"/>
-      <c r="P28" s="178"/>
+      <c r="A28" s="177"/>
+      <c r="B28" s="168"/>
+      <c r="C28" s="162"/>
+      <c r="D28" s="162"/>
+      <c r="E28" s="162"/>
+      <c r="F28" s="162"/>
+      <c r="G28" s="162"/>
+      <c r="H28" s="162"/>
+      <c r="I28" s="162"/>
+      <c r="J28" s="162"/>
+      <c r="K28" s="162"/>
+      <c r="L28" s="162"/>
+      <c r="M28" s="162"/>
+      <c r="N28" s="162"/>
+      <c r="O28" s="162"/>
+      <c r="P28" s="177"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="178"/>
-      <c r="B29" s="169"/>
-      <c r="C29" s="161"/>
-      <c r="D29" s="161"/>
-      <c r="E29" s="161"/>
-      <c r="F29" s="161"/>
-      <c r="G29" s="161"/>
-      <c r="H29" s="161"/>
-      <c r="I29" s="161"/>
-      <c r="J29" s="161"/>
-      <c r="K29" s="161"/>
-      <c r="L29" s="161"/>
-      <c r="M29" s="161"/>
-      <c r="N29" s="161"/>
-      <c r="O29" s="161"/>
-      <c r="P29" s="178"/>
+      <c r="A29" s="177"/>
+      <c r="B29" s="168"/>
+      <c r="C29" s="160"/>
+      <c r="D29" s="160"/>
+      <c r="E29" s="160"/>
+      <c r="F29" s="160"/>
+      <c r="G29" s="160"/>
+      <c r="H29" s="160"/>
+      <c r="I29" s="160"/>
+      <c r="J29" s="160"/>
+      <c r="K29" s="160"/>
+      <c r="L29" s="160"/>
+      <c r="M29" s="160"/>
+      <c r="N29" s="160"/>
+      <c r="O29" s="160"/>
+      <c r="P29" s="177"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="178"/>
-      <c r="B30" s="178"/>
-      <c r="C30" s="178"/>
-      <c r="D30" s="178"/>
-      <c r="E30" s="178"/>
-      <c r="F30" s="178"/>
-      <c r="G30" s="178"/>
-      <c r="H30" s="178"/>
-      <c r="I30" s="178"/>
-      <c r="J30" s="178"/>
-      <c r="K30" s="178"/>
-      <c r="L30" s="178"/>
-      <c r="M30" s="178"/>
-      <c r="N30" s="178"/>
-      <c r="O30" s="178"/>
-      <c r="P30" s="178"/>
+      <c r="A30" s="177"/>
+      <c r="B30" s="177"/>
+      <c r="C30" s="177"/>
+      <c r="D30" s="177"/>
+      <c r="E30" s="177"/>
+      <c r="F30" s="177"/>
+      <c r="G30" s="177"/>
+      <c r="H30" s="177"/>
+      <c r="I30" s="177"/>
+      <c r="J30" s="177"/>
+      <c r="K30" s="177"/>
+      <c r="L30" s="177"/>
+      <c r="M30" s="177"/>
+      <c r="N30" s="177"/>
+      <c r="O30" s="177"/>
+      <c r="P30" s="177"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="178"/>
-      <c r="B31" s="169"/>
-      <c r="C31" s="169"/>
-      <c r="D31" s="169"/>
-      <c r="E31" s="169"/>
-      <c r="F31" s="169"/>
-      <c r="G31" s="169"/>
-      <c r="H31" s="169"/>
-      <c r="I31" s="169"/>
-      <c r="J31" s="169"/>
-      <c r="K31" s="169"/>
-      <c r="L31" s="169"/>
-      <c r="M31" s="169"/>
-      <c r="N31" s="169"/>
-      <c r="O31" s="169"/>
-      <c r="P31" s="178"/>
+      <c r="A31" s="177"/>
+      <c r="B31" s="168"/>
+      <c r="C31" s="168"/>
+      <c r="D31" s="168"/>
+      <c r="E31" s="168"/>
+      <c r="F31" s="168"/>
+      <c r="G31" s="168"/>
+      <c r="H31" s="168"/>
+      <c r="I31" s="168"/>
+      <c r="J31" s="168"/>
+      <c r="K31" s="168"/>
+      <c r="L31" s="168"/>
+      <c r="M31" s="168"/>
+      <c r="N31" s="168"/>
+      <c r="O31" s="168"/>
+      <c r="P31" s="177"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="178"/>
-      <c r="B32" s="163"/>
-      <c r="C32" s="163"/>
-      <c r="D32" s="163"/>
-      <c r="E32" s="174"/>
-      <c r="F32" s="181"/>
-      <c r="G32" s="163"/>
-      <c r="H32" s="163"/>
-      <c r="I32" s="175"/>
-      <c r="J32" s="182"/>
-      <c r="K32" s="176"/>
-      <c r="L32" s="183"/>
-      <c r="M32" s="184"/>
-      <c r="N32" s="184"/>
-      <c r="O32" s="165"/>
-      <c r="P32" s="178"/>
+      <c r="A32" s="177"/>
+      <c r="B32" s="162"/>
+      <c r="C32" s="162"/>
+      <c r="D32" s="162"/>
+      <c r="E32" s="173"/>
+      <c r="F32" s="180"/>
+      <c r="G32" s="162"/>
+      <c r="H32" s="162"/>
+      <c r="I32" s="174"/>
+      <c r="J32" s="181"/>
+      <c r="K32" s="175"/>
+      <c r="L32" s="182"/>
+      <c r="M32" s="183"/>
+      <c r="N32" s="183"/>
+      <c r="O32" s="164"/>
+      <c r="P32" s="177"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A33" s="178"/>
-      <c r="B33" s="169"/>
-      <c r="C33" s="169"/>
-      <c r="D33" s="169"/>
-      <c r="E33" s="169"/>
-      <c r="F33" s="169"/>
-      <c r="G33" s="169"/>
-      <c r="H33" s="169"/>
-      <c r="I33" s="169"/>
-      <c r="J33" s="169"/>
-      <c r="K33" s="169"/>
-      <c r="L33" s="169"/>
-      <c r="M33" s="169"/>
-      <c r="N33" s="185"/>
-      <c r="O33" s="186"/>
-      <c r="P33" s="178"/>
+      <c r="A33" s="177"/>
+      <c r="B33" s="168"/>
+      <c r="C33" s="168"/>
+      <c r="D33" s="168"/>
+      <c r="E33" s="168"/>
+      <c r="F33" s="168"/>
+      <c r="G33" s="168"/>
+      <c r="H33" s="168"/>
+      <c r="I33" s="168"/>
+      <c r="J33" s="168"/>
+      <c r="K33" s="168"/>
+      <c r="L33" s="168"/>
+      <c r="M33" s="168"/>
+      <c r="N33" s="184"/>
+      <c r="O33" s="185"/>
+      <c r="P33" s="177"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A34" s="178"/>
-      <c r="B34" s="178"/>
-      <c r="C34" s="178"/>
-      <c r="D34" s="178"/>
-      <c r="E34" s="178"/>
-      <c r="F34" s="178"/>
-      <c r="G34" s="178"/>
-      <c r="H34" s="178"/>
-      <c r="I34" s="178"/>
-      <c r="J34" s="178"/>
-      <c r="K34" s="178"/>
-      <c r="L34" s="178"/>
-      <c r="M34" s="178"/>
-      <c r="N34" s="178"/>
-      <c r="O34" s="178"/>
-      <c r="P34" s="178"/>
+      <c r="A34" s="177"/>
+      <c r="B34" s="177"/>
+      <c r="C34" s="177"/>
+      <c r="D34" s="177"/>
+      <c r="E34" s="177"/>
+      <c r="F34" s="177"/>
+      <c r="G34" s="177"/>
+      <c r="H34" s="177"/>
+      <c r="I34" s="177"/>
+      <c r="J34" s="177"/>
+      <c r="K34" s="177"/>
+      <c r="L34" s="177"/>
+      <c r="M34" s="177"/>
+      <c r="N34" s="177"/>
+      <c r="O34" s="177"/>
+      <c r="P34" s="177"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A35" s="178"/>
-      <c r="B35" s="169"/>
-      <c r="C35" s="169"/>
-      <c r="D35" s="169"/>
-      <c r="E35" s="169"/>
-      <c r="F35" s="169"/>
-      <c r="G35" s="169"/>
-      <c r="H35" s="169"/>
-      <c r="I35" s="169"/>
-      <c r="J35" s="169"/>
-      <c r="K35" s="169"/>
-      <c r="L35" s="169"/>
-      <c r="M35" s="169"/>
-      <c r="N35" s="169"/>
-      <c r="O35" s="169"/>
-      <c r="P35" s="178"/>
+      <c r="A35" s="177"/>
+      <c r="B35" s="168"/>
+      <c r="C35" s="168"/>
+      <c r="D35" s="168"/>
+      <c r="E35" s="168"/>
+      <c r="F35" s="168"/>
+      <c r="G35" s="168"/>
+      <c r="H35" s="168"/>
+      <c r="I35" s="168"/>
+      <c r="J35" s="168"/>
+      <c r="K35" s="168"/>
+      <c r="L35" s="168"/>
+      <c r="M35" s="168"/>
+      <c r="N35" s="168"/>
+      <c r="O35" s="168"/>
+      <c r="P35" s="177"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A36" s="178"/>
-      <c r="B36" s="163"/>
-      <c r="C36" s="177"/>
-      <c r="D36" s="187"/>
-      <c r="E36" s="174"/>
-      <c r="F36" s="163"/>
-      <c r="G36" s="163"/>
-      <c r="H36" s="173"/>
-      <c r="I36" s="188"/>
-      <c r="J36" s="174"/>
-      <c r="K36" s="161"/>
-      <c r="L36" s="161"/>
-      <c r="M36" s="161"/>
-      <c r="N36" s="161"/>
-      <c r="O36" s="161"/>
-      <c r="P36" s="178"/>
+      <c r="A36" s="177"/>
+      <c r="B36" s="162"/>
+      <c r="C36" s="176"/>
+      <c r="D36" s="186"/>
+      <c r="E36" s="173"/>
+      <c r="F36" s="162"/>
+      <c r="G36" s="162"/>
+      <c r="H36" s="172"/>
+      <c r="I36" s="187"/>
+      <c r="J36" s="173"/>
+      <c r="K36" s="160"/>
+      <c r="L36" s="160"/>
+      <c r="M36" s="160"/>
+      <c r="N36" s="160"/>
+      <c r="O36" s="160"/>
+      <c r="P36" s="177"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A37" s="178"/>
-      <c r="B37" s="163"/>
-      <c r="C37" s="177"/>
-      <c r="D37" s="187"/>
-      <c r="E37" s="174"/>
-      <c r="F37" s="163"/>
-      <c r="G37" s="188"/>
-      <c r="H37" s="173"/>
-      <c r="I37" s="163"/>
-      <c r="J37" s="174"/>
-      <c r="K37" s="161"/>
-      <c r="L37" s="161"/>
-      <c r="M37" s="161"/>
-      <c r="N37" s="161"/>
-      <c r="O37" s="161"/>
-      <c r="P37" s="178"/>
+      <c r="A37" s="177"/>
+      <c r="B37" s="162"/>
+      <c r="C37" s="176"/>
+      <c r="D37" s="186"/>
+      <c r="E37" s="173"/>
+      <c r="F37" s="162"/>
+      <c r="G37" s="187"/>
+      <c r="H37" s="172"/>
+      <c r="I37" s="162"/>
+      <c r="J37" s="173"/>
+      <c r="K37" s="160"/>
+      <c r="L37" s="160"/>
+      <c r="M37" s="160"/>
+      <c r="N37" s="160"/>
+      <c r="O37" s="160"/>
+      <c r="P37" s="177"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A38" s="178"/>
-      <c r="B38" s="169"/>
-      <c r="C38" s="169"/>
-      <c r="D38" s="169"/>
-      <c r="E38" s="169"/>
-      <c r="F38" s="169"/>
-      <c r="G38" s="169"/>
-      <c r="H38" s="169"/>
-      <c r="I38" s="185"/>
-      <c r="J38" s="186"/>
-      <c r="K38" s="169"/>
-      <c r="L38" s="169"/>
-      <c r="M38" s="169"/>
-      <c r="N38" s="169"/>
-      <c r="O38" s="169"/>
-      <c r="P38" s="178"/>
+      <c r="A38" s="177"/>
+      <c r="B38" s="168"/>
+      <c r="C38" s="168"/>
+      <c r="D38" s="168"/>
+      <c r="E38" s="168"/>
+      <c r="F38" s="168"/>
+      <c r="G38" s="168"/>
+      <c r="H38" s="168"/>
+      <c r="I38" s="184"/>
+      <c r="J38" s="185"/>
+      <c r="K38" s="168"/>
+      <c r="L38" s="168"/>
+      <c r="M38" s="168"/>
+      <c r="N38" s="168"/>
+      <c r="O38" s="168"/>
+      <c r="P38" s="177"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A39" s="178"/>
-      <c r="B39" s="161"/>
-      <c r="C39" s="161"/>
-      <c r="D39" s="161"/>
-      <c r="E39" s="161"/>
-      <c r="F39" s="161"/>
-      <c r="G39" s="161"/>
-      <c r="H39" s="161"/>
-      <c r="I39" s="164"/>
-      <c r="J39" s="170"/>
-      <c r="K39" s="161"/>
-      <c r="L39" s="163"/>
-      <c r="M39" s="163"/>
-      <c r="N39" s="163"/>
-      <c r="O39" s="163"/>
-      <c r="P39" s="178"/>
+      <c r="A39" s="177"/>
+      <c r="B39" s="160"/>
+      <c r="C39" s="160"/>
+      <c r="D39" s="160"/>
+      <c r="E39" s="160"/>
+      <c r="F39" s="160"/>
+      <c r="G39" s="160"/>
+      <c r="H39" s="160"/>
+      <c r="I39" s="163"/>
+      <c r="J39" s="169"/>
+      <c r="K39" s="160"/>
+      <c r="L39" s="162"/>
+      <c r="M39" s="162"/>
+      <c r="N39" s="162"/>
+      <c r="O39" s="162"/>
+      <c r="P39" s="177"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B40" s="172"/>
-      <c r="C40" s="172"/>
-      <c r="D40" s="172"/>
-      <c r="E40" s="172"/>
-      <c r="F40" s="172"/>
-      <c r="G40" s="172"/>
-      <c r="H40" s="172"/>
-      <c r="I40" s="172"/>
-      <c r="J40" s="172"/>
-      <c r="K40" s="172"/>
-      <c r="L40" s="172"/>
-      <c r="M40" s="172"/>
-      <c r="N40" s="172"/>
-      <c r="O40" s="172"/>
+      <c r="B40" s="171"/>
+      <c r="C40" s="171"/>
+      <c r="D40" s="171"/>
+      <c r="E40" s="171"/>
+      <c r="F40" s="171"/>
+      <c r="G40" s="171"/>
+      <c r="H40" s="171"/>
+      <c r="I40" s="171"/>
+      <c r="J40" s="171"/>
+      <c r="K40" s="171"/>
+      <c r="L40" s="171"/>
+      <c r="M40" s="171"/>
+      <c r="N40" s="171"/>
+      <c r="O40" s="171"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>